<commit_message>
nxp ble sdk 分析
</commit_message>
<xml_diff>
--- a/Gavin_OBS/英语/Alphabet/A词汇表.xlsx
+++ b/Gavin_OBS/英语/Alphabet/A词汇表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NXF91053\Documents\Gavin_OBS\Gavin_OBS\英语\Alphabet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF280B1-0A16-4BE1-81D6-0A4866E91D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0116D4D0-C05C-44DF-8DEB-C8AB5BD87686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{6D76B9EA-1B1F-447C-BB05-A4DDD04CA0AD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{6D76B9EA-1B1F-447C-BB05-A4DDD04CA0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="736">
   <si>
     <t>单词</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2950,6 +2951,62 @@
   </si>
   <si>
     <t>警察</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>are you a doctor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hospital</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>farmer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cleaner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>painter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hurt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>healthy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>building</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>names of parts of our body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shoulders</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>head</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4423,6 +4480,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A115:F115"/>
+    <mergeCell ref="A116:A127"/>
+    <mergeCell ref="D116:D127"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="D133:D143"/>
+    <mergeCell ref="A133:A143"/>
     <mergeCell ref="A98:F98"/>
     <mergeCell ref="D99:D110"/>
     <mergeCell ref="A99:A110"/>
@@ -4436,12 +4499,6 @@
     <mergeCell ref="A79:F79"/>
     <mergeCell ref="A80:A92"/>
     <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A115:F115"/>
-    <mergeCell ref="A116:A127"/>
-    <mergeCell ref="D116:D127"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="D133:D143"/>
-    <mergeCell ref="A133:A143"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5382,6 +5439,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A86:A96"/>
+    <mergeCell ref="D86:D96"/>
+    <mergeCell ref="A101:F101"/>
+    <mergeCell ref="A102:A113"/>
+    <mergeCell ref="D102:D113"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="D70:D80"/>
+    <mergeCell ref="A70:A80"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:A64"/>
+    <mergeCell ref="D52:D64"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="D2:D14"/>
@@ -5391,18 +5460,6 @@
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A20:A31"/>
     <mergeCell ref="D20:D31"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="D70:D80"/>
-    <mergeCell ref="A70:A80"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:A64"/>
-    <mergeCell ref="D52:D64"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="A86:A96"/>
-    <mergeCell ref="D86:D96"/>
-    <mergeCell ref="A101:F101"/>
-    <mergeCell ref="A102:A113"/>
-    <mergeCell ref="D102:D113"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6496,13 +6553,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="D20:D26"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="D2:D15"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A124:A135"/>
+    <mergeCell ref="D124:D135"/>
+    <mergeCell ref="A90:A100"/>
+    <mergeCell ref="D90:D100"/>
+    <mergeCell ref="A105:F105"/>
+    <mergeCell ref="A106:A117"/>
+    <mergeCell ref="D106:D117"/>
     <mergeCell ref="A68:F68"/>
     <mergeCell ref="A69:A84"/>
     <mergeCell ref="D69:D84"/>
@@ -6512,14 +6570,13 @@
     <mergeCell ref="A50:F50"/>
     <mergeCell ref="A51:A63"/>
     <mergeCell ref="D51:D63"/>
-    <mergeCell ref="A123:F123"/>
-    <mergeCell ref="A124:A135"/>
-    <mergeCell ref="D124:D135"/>
-    <mergeCell ref="A90:A100"/>
-    <mergeCell ref="D90:D100"/>
-    <mergeCell ref="A105:F105"/>
-    <mergeCell ref="A106:A117"/>
-    <mergeCell ref="D106:D117"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="D20:D26"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="D2:D15"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7631,7 +7688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8393AF72-B4E8-4F23-93D4-3ED00FB677F0}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
@@ -8079,4 +8136,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9500599E-60E8-463B-994C-9C91EE191784}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>723</v>
+      </c>
+      <c r="C2" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2" t="s">
+        <v>730</v>
+      </c>
+      <c r="E2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>727</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>735</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>